<commit_message>
feat: Added quarterly and yearly goals to project-management.xlsx
</commit_message>
<xml_diff>
--- a/project-management.xlsx
+++ b/project-management.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="594" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Week</t>
   </si>
@@ -66,6 +66,33 @@
   </si>
   <si>
     <t>Complete fully automated CI / CD</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>1st quarter</t>
+  </si>
+  <si>
+    <t>2nd quarter</t>
+  </si>
+  <si>
+    <t>3rd quarter</t>
+  </si>
+  <si>
+    <t>4th quarter</t>
+  </si>
+  <si>
+    <t>Gather data from the market, get data from all stakeholders</t>
+  </si>
+  <si>
+    <t>Build the ML backend using Flask</t>
+  </si>
+  <si>
+    <t>Build the FE using Vue.js</t>
+  </si>
+  <si>
+    <t>Deliver to production San Francisto's house predictions using fully automated CI / CD</t>
   </si>
 </sst>
 </file>
@@ -305,18 +332,20 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6479591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4540816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="70.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,6 +825,40 @@
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
     </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>